<commit_message>
Made the code make sure the simulation isn't already in the spreadsheet
</commit_message>
<xml_diff>
--- a/NestedBinaryData.xlsx
+++ b/NestedBinaryData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminkhoury/Documents/GitHub/AstroResearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37BE334-ABDC-AE4E-A3DB-9944CD4FCD8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18EFB3F-7EDD-1A41-9AB2-A77B19AFDB55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15920" xr2:uid="{FDF47A62-6035-1E46-A9DF-7E3B179B0102}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>m1</t>
   </si>
@@ -490,7 +490,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,7 +502,7 @@
     <col min="17" max="17" width="42.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,32 +533,32 @@
       <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s" s="1">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s" s="1">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s" s="1">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s" s="1">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" t="s" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Fixed syntax Added file which fixes m's and a's but rotates m3 made period default 1000P everywhere Added Kate's file
</commit_message>
<xml_diff>
--- a/NestedBinaryData.xlsx
+++ b/NestedBinaryData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="633">
   <si>
     <t>m1</t>
   </si>
@@ -1678,6 +1678,342 @@
   </si>
   <si>
     <t>[0.002027504438193837,0.0034193896880718327]</t>
+  </si>
+  <si>
+    <t>1000P periods</t>
+  </si>
+  <si>
+    <t>[-6.046939064287374e-11,2.970806695705539e-12]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,975.641655082653],[0.0,0.0,975.6416551017463]]</t>
+  </si>
+  <si>
+    <t>[-3614.95414535744,-2883.718844549143]</t>
+  </si>
+  <si>
+    <t>[-1337.228393030528,-829.3502517782138]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,0.0],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[0.0004563137537233886,0.0008053631485530542]</t>
+  </si>
+  <si>
+    <t>[-3.007353937740412e-11,1.3955310207952258e-9]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,1000.2004065221081],[0.0,0.0,1000.2004069523357]]</t>
+  </si>
+  <si>
+    <t>[-3565.693567912392,-2815.9767215302654]</t>
+  </si>
+  <si>
+    <t>[-1202.920629494612,-722.5493307063912]</t>
+  </si>
+  <si>
+    <t>[0.0004564579821494023,0.0008063666218747724]</t>
+  </si>
+  <si>
+    <t>[0.0,1.2456245400627403e-7]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,4896.126236248317],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2293.985269926886,-2260.6389730146825]</t>
+  </si>
+  <si>
+    <t>[-169.95291397371298,-65.60678614472278]</t>
+  </si>
+  <si>
+    <t>[0.00626711358588136,0.006471667054336739]</t>
+  </si>
+  <si>
+    <t>[-1.2669332101872325e-11,9.827117504271895e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,4536.001800930624],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2515.245289129506,-2260.7145887270026]</t>
+  </si>
+  <si>
+    <t>[-176.41908955386344,123.6320244138613]</t>
+  </si>
+  <si>
+    <t>[0.004259098964354781,0.007403528731528524]</t>
+  </si>
+  <si>
+    <t>[0.0,2.5104293858477443e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,3593.183258829851],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2291.7976697123177,-2265.004858314624]</t>
+  </si>
+  <si>
+    <t>[-159.37230699154404,-81.68773353013063]</t>
+  </si>
+  <si>
+    <t>[0.006352710121004197,0.006432902849153114]</t>
+  </si>
+  <si>
+    <t>[0.0,2.218291291511624e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,2427.795450191914],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2289.653212833143,-2266.9510030633082]</t>
+  </si>
+  <si>
+    <t>[-148.2255842134629,-79.02619095378725]</t>
+  </si>
+  <si>
+    <t>[0.006366689520028675,0.006445856707297158]</t>
+  </si>
+  <si>
+    <t>[0.0,2.466204295477768e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,1484.9769079579821],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2287.6028431838313,-2262.423348552621]</t>
+  </si>
+  <si>
+    <t>[-150.6043089222757,-73.46478623816222]</t>
+  </si>
+  <si>
+    <t>[0.006367392989904797,0.0064562850847207755]</t>
+  </si>
+  <si>
+    <t>[0.0,1.2377466136566902e-7]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,1124.852068124762],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2285.197192732333,-2253.91836480807]</t>
+  </si>
+  <si>
+    <t>[-169.52755173827566,-65.42887438694277]</t>
+  </si>
+  <si>
+    <t>[0.00634722009269794,0.006470293908743449]</t>
+  </si>
+  <si>
+    <t>[-6.0498831134854026e-12,3.547338094843459e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,1484.9769079164403],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2321.5754937581646,-2217.0744717227403]</t>
+  </si>
+  <si>
+    <t>[-201.97002151694699,6.878024739128932]</t>
+  </si>
+  <si>
+    <t>[0.0043391092500468555,0.006690378662341604]</t>
+  </si>
+  <si>
+    <t>[-9.150420288664775e-10,9.477443016957469e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,2427.7954501909057],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-3420.1231167807955,-1823.9820839116078]</t>
+  </si>
+  <si>
+    <t>[-1248.070538397003,5722.8847488173415]</t>
+  </si>
+  <si>
+    <t>[0.0001737438445264283,0.010567012128438384]</t>
+  </si>
+  <si>
+    <t>[-1.186851579098434e-5,6.02514504985459e-12]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,3593.1832565132036],[0.0,0.0,3593.18325926986]]</t>
+  </si>
+  <si>
+    <t>[-3901.034616056694,3.566423595983679e6]</t>
+  </si>
+  <si>
+    <t>[-2738.706803962937,6.271900045101356e7]</t>
+  </si>
+  <si>
+    <t>[2.771850425589169e-10,0.028948795598466654]</t>
+  </si>
+  <si>
+    <t>[-7.831839217506987e-11,1.0010993407217755e-10]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,4536.001801017598],[0.0,0.0,4536.001801139413]]</t>
+  </si>
+  <si>
+    <t>[-2328.1472858283423,-2138.680316676339]</t>
+  </si>
+  <si>
+    <t>[-189.86396520111043,-66.40182835263852]</t>
+  </si>
+  <si>
+    <t>[0.003790278375165637,0.010040638685672277]</t>
+  </si>
+  <si>
+    <t>[0.0,1.2448868410042784e-7]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,4896.126236312554],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2292.988654749074,-2260.1833513537367]</t>
+  </si>
+  <si>
+    <t>[-170.10631252411568,-65.91486758054157]</t>
+  </si>
+  <si>
+    <t>[0.0062884227062314745,0.00645679802781983]</t>
+  </si>
+  <si>
+    <t>[-4.109655657185108e-11,9.70258706813093e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,4536.001800926036],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2541.344407412897,-2224.2828633117965]</t>
+  </si>
+  <si>
+    <t>[-199.7164296243186,268.16226216064877]</t>
+  </si>
+  <si>
+    <t>[0.003958283722565165,0.007558335328314811]</t>
+  </si>
+  <si>
+    <t>[0.0,2.3899284405576858e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,3593.1832588324605],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2289.46216649518,-2269.3968472689203]</t>
+  </si>
+  <si>
+    <t>[-153.28654634529408,-77.84794638968998]</t>
+  </si>
+  <si>
+    <t>[0.0063565851873717,0.006427074734661797]</t>
+  </si>
+  <si>
+    <t>[-5.354094341634495e-16,2.1845954202548454e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,2427.7954501923646],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2286.1181496617564,-2264.697404030584]</t>
+  </si>
+  <si>
+    <t>[-158.08098103415045,-86.75434269438702]</t>
+  </si>
+  <si>
+    <t>[0.006371473312929187,0.006439419774935288]</t>
+  </si>
+  <si>
+    <t>[0.0,2.4604275010558124e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,1484.9769079581934],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2285.005000838378,-2258.9631270010527]</t>
+  </si>
+  <si>
+    <t>[-162.51945969096712,-82.68058198699418]</t>
+  </si>
+  <si>
+    <t>[0.00637238166606447,0.006450803221022618]</t>
+  </si>
+  <si>
+    <t>[0.0,1.237748332547009e-7]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,1124.8520681243645],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2285.201589598474,-2253.9102714264836]</t>
+  </si>
+  <si>
+    <t>[-169.53155531179323,-65.42927959465982]</t>
+  </si>
+  <si>
+    <t>[0.006347217617245445,0.006470293264954129]</t>
+  </si>
+  <si>
+    <t>[-5.048162638722419e-12,4.486952003121774e-11]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,1484.9769079265357],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-2318.57575146697,-2210.1568775996516]</t>
+  </si>
+  <si>
+    <t>[-205.1847662041149,8.908601259719717]</t>
+  </si>
+  <si>
+    <t>[0.004172736119501224,0.006719477100050219]</t>
+  </si>
+  <si>
+    <t>[-1.263498438675084e-8,2.435542761871689e-9]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,2427.795450201531],[0.0,0.0,0.0]]</t>
+  </si>
+  <si>
+    <t>[-4396.694968905555,3961.632725953993]</t>
+  </si>
+  <si>
+    <t>[-178.53358453896806,79593.0331922949]</t>
+  </si>
+  <si>
+    <t>[3.685192182672663e-6,0.016408017683696045]</t>
+  </si>
+  <si>
+    <t>[-5.453272901181741e-9,6.509055503606367e-12]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,3593.1832587224185],[0.0,0.0,3593.1832588825578]]</t>
+  </si>
+  <si>
+    <t>[-4130.613873885532,-644.2667513599572]</t>
+  </si>
+  <si>
+    <t>[-12709.623409818627,31033.456904803228]</t>
+  </si>
+  <si>
+    <t>[2.4410402403405182e-5,0.01221844492107093]</t>
+  </si>
+  <si>
+    <t>[-2.041130984977972e-10,1.299985655318103e-10]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,4536.001801003193],[0.0,0.0,4536.001801115255]]</t>
+  </si>
+  <si>
+    <t>[-2541.2525393865217,-2032.2190949835544]</t>
+  </si>
+  <si>
+    <t>[-336.83500835198697,329.25982684066446]</t>
+  </si>
+  <si>
+    <t>[0.0023328370399377293,0.011461353231489195]</t>
   </si>
 </sst>
 </file>
@@ -2095,7 +2431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE073501-CAF1-7547-9F20-DE970FECDDD2}">
-  <dimension ref="A1:W72"/>
+  <dimension ref="A1:W94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
@@ -7225,6 +7561,1568 @@
       </c>
       <c r="W72">
         <v>251897</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23">
+      <c r="A73">
+        <v>8.0</v>
+      </c>
+      <c r="B73">
+        <v>1.5</v>
+      </c>
+      <c r="C73">
+        <v>1.0</v>
+      </c>
+      <c r="D73">
+        <v>5.0</v>
+      </c>
+      <c r="E73">
+        <v>0.0</v>
+      </c>
+      <c r="F73">
+        <v>10.0</v>
+      </c>
+      <c r="G73">
+        <v>0.0</v>
+      </c>
+      <c r="H73">
+        <v>0.0</v>
+      </c>
+      <c r="I73">
+        <v>0.0</v>
+      </c>
+      <c r="J73" t="s">
+        <v>521</v>
+      </c>
+      <c r="K73">
+        <v>0.01</v>
+      </c>
+      <c r="L73" t="s">
+        <v>522</v>
+      </c>
+      <c r="M73" t="s">
+        <v>523</v>
+      </c>
+      <c r="N73" t="s">
+        <v>524</v>
+      </c>
+      <c r="O73" t="s">
+        <v>525</v>
+      </c>
+      <c r="P73" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>526</v>
+      </c>
+      <c r="R73">
+        <v>0.12307000160217285</v>
+      </c>
+      <c r="S73" t="s">
+        <v>527</v>
+      </c>
+      <c r="T73">
+        <v>0</v>
+      </c>
+      <c r="U73">
+        <v>73</v>
+      </c>
+      <c r="V73">
+        <v>1</v>
+      </c>
+      <c r="W73">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23">
+      <c r="A74">
+        <v>8.0</v>
+      </c>
+      <c r="B74">
+        <v>1.5</v>
+      </c>
+      <c r="C74">
+        <v>1.0</v>
+      </c>
+      <c r="D74">
+        <v>5.0</v>
+      </c>
+      <c r="E74">
+        <v>0.0</v>
+      </c>
+      <c r="F74">
+        <v>11.0</v>
+      </c>
+      <c r="G74">
+        <v>0.0</v>
+      </c>
+      <c r="H74">
+        <v>0.0</v>
+      </c>
+      <c r="I74">
+        <v>0.0</v>
+      </c>
+      <c r="J74" t="s">
+        <v>521</v>
+      </c>
+      <c r="K74">
+        <v>0.01</v>
+      </c>
+      <c r="L74" t="s">
+        <v>528</v>
+      </c>
+      <c r="M74" t="s">
+        <v>529</v>
+      </c>
+      <c r="N74" t="s">
+        <v>530</v>
+      </c>
+      <c r="O74" t="s">
+        <v>531</v>
+      </c>
+      <c r="P74" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>526</v>
+      </c>
+      <c r="R74">
+        <v>1.2333011627197266</v>
+      </c>
+      <c r="S74" t="s">
+        <v>532</v>
+      </c>
+      <c r="T74">
+        <v>0</v>
+      </c>
+      <c r="U74">
+        <v>74</v>
+      </c>
+      <c r="V74">
+        <v>1</v>
+      </c>
+      <c r="W74">
+        <v>65728</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23">
+      <c r="A75">
+        <v>8.0</v>
+      </c>
+      <c r="B75">
+        <v>5.0</v>
+      </c>
+      <c r="C75">
+        <v>1.0</v>
+      </c>
+      <c r="D75">
+        <v>25.0</v>
+      </c>
+      <c r="E75">
+        <v>0.0</v>
+      </c>
+      <c r="F75">
+        <v>100.0</v>
+      </c>
+      <c r="G75">
+        <v>0.0</v>
+      </c>
+      <c r="H75">
+        <v>0.0</v>
+      </c>
+      <c r="I75">
+        <v>0.0</v>
+      </c>
+      <c r="J75" t="s">
+        <v>521</v>
+      </c>
+      <c r="K75">
+        <v>0.01</v>
+      </c>
+      <c r="L75" t="s">
+        <v>533</v>
+      </c>
+      <c r="M75" t="s">
+        <v>534</v>
+      </c>
+      <c r="N75" t="s">
+        <v>535</v>
+      </c>
+      <c r="O75" t="s">
+        <v>536</v>
+      </c>
+      <c r="P75" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>526</v>
+      </c>
+      <c r="R75">
+        <v>79.03585505485535</v>
+      </c>
+      <c r="S75" t="s">
+        <v>537</v>
+      </c>
+      <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="U75">
+        <v>75</v>
+      </c>
+      <c r="V75">
+        <v>1</v>
+      </c>
+      <c r="W75">
+        <v>4854461</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23">
+      <c r="A76">
+        <v>8.0</v>
+      </c>
+      <c r="B76">
+        <v>5.0</v>
+      </c>
+      <c r="C76">
+        <v>1.0</v>
+      </c>
+      <c r="D76">
+        <v>25.0</v>
+      </c>
+      <c r="E76">
+        <v>0.0</v>
+      </c>
+      <c r="F76">
+        <v>100.0</v>
+      </c>
+      <c r="G76">
+        <v>0.0</v>
+      </c>
+      <c r="H76">
+        <v>18.0</v>
+      </c>
+      <c r="I76">
+        <v>0.0</v>
+      </c>
+      <c r="J76" t="s">
+        <v>521</v>
+      </c>
+      <c r="K76">
+        <v>0.01</v>
+      </c>
+      <c r="L76" t="s">
+        <v>538</v>
+      </c>
+      <c r="M76" t="s">
+        <v>539</v>
+      </c>
+      <c r="N76" t="s">
+        <v>540</v>
+      </c>
+      <c r="O76" t="s">
+        <v>541</v>
+      </c>
+      <c r="P76" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>526</v>
+      </c>
+      <c r="R76">
+        <v>0.11619305610656738</v>
+      </c>
+      <c r="S76" t="s">
+        <v>542</v>
+      </c>
+      <c r="T76">
+        <v>0</v>
+      </c>
+      <c r="U76">
+        <v>76</v>
+      </c>
+      <c r="V76">
+        <v>1</v>
+      </c>
+      <c r="W76">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23">
+      <c r="A77">
+        <v>8.0</v>
+      </c>
+      <c r="B77">
+        <v>5.0</v>
+      </c>
+      <c r="C77">
+        <v>1.0</v>
+      </c>
+      <c r="D77">
+        <v>25.0</v>
+      </c>
+      <c r="E77">
+        <v>0.0</v>
+      </c>
+      <c r="F77">
+        <v>100.0</v>
+      </c>
+      <c r="G77">
+        <v>0.0</v>
+      </c>
+      <c r="H77">
+        <v>36.0</v>
+      </c>
+      <c r="I77">
+        <v>0.0</v>
+      </c>
+      <c r="J77" t="s">
+        <v>521</v>
+      </c>
+      <c r="K77">
+        <v>0.01</v>
+      </c>
+      <c r="L77" t="s">
+        <v>543</v>
+      </c>
+      <c r="M77" t="s">
+        <v>544</v>
+      </c>
+      <c r="N77" t="s">
+        <v>545</v>
+      </c>
+      <c r="O77" t="s">
+        <v>546</v>
+      </c>
+      <c r="P77" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>526</v>
+      </c>
+      <c r="R77">
+        <v>0.02109217643737793</v>
+      </c>
+      <c r="S77" t="s">
+        <v>547</v>
+      </c>
+      <c r="T77">
+        <v>0</v>
+      </c>
+      <c r="U77">
+        <v>77</v>
+      </c>
+      <c r="V77">
+        <v>1</v>
+      </c>
+      <c r="W77">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23">
+      <c r="A78">
+        <v>8.0</v>
+      </c>
+      <c r="B78">
+        <v>5.0</v>
+      </c>
+      <c r="C78">
+        <v>1.0</v>
+      </c>
+      <c r="D78">
+        <v>25.0</v>
+      </c>
+      <c r="E78">
+        <v>0.0</v>
+      </c>
+      <c r="F78">
+        <v>100.0</v>
+      </c>
+      <c r="G78">
+        <v>0.0</v>
+      </c>
+      <c r="H78">
+        <v>54.0</v>
+      </c>
+      <c r="I78">
+        <v>0.0</v>
+      </c>
+      <c r="J78" t="s">
+        <v>521</v>
+      </c>
+      <c r="K78">
+        <v>0.01</v>
+      </c>
+      <c r="L78" t="s">
+        <v>548</v>
+      </c>
+      <c r="M78" t="s">
+        <v>549</v>
+      </c>
+      <c r="N78" t="s">
+        <v>550</v>
+      </c>
+      <c r="O78" t="s">
+        <v>551</v>
+      </c>
+      <c r="P78" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>526</v>
+      </c>
+      <c r="R78">
+        <v>0.019444942474365234</v>
+      </c>
+      <c r="S78" t="s">
+        <v>552</v>
+      </c>
+      <c r="T78">
+        <v>0</v>
+      </c>
+      <c r="U78">
+        <v>78</v>
+      </c>
+      <c r="V78">
+        <v>1</v>
+      </c>
+      <c r="W78">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23">
+      <c r="A79">
+        <v>8.0</v>
+      </c>
+      <c r="B79">
+        <v>5.0</v>
+      </c>
+      <c r="C79">
+        <v>1.0</v>
+      </c>
+      <c r="D79">
+        <v>25.0</v>
+      </c>
+      <c r="E79">
+        <v>0.0</v>
+      </c>
+      <c r="F79">
+        <v>100.0</v>
+      </c>
+      <c r="G79">
+        <v>0.0</v>
+      </c>
+      <c r="H79">
+        <v>72.0</v>
+      </c>
+      <c r="I79">
+        <v>0.0</v>
+      </c>
+      <c r="J79" t="s">
+        <v>521</v>
+      </c>
+      <c r="K79">
+        <v>0.01</v>
+      </c>
+      <c r="L79" t="s">
+        <v>553</v>
+      </c>
+      <c r="M79" t="s">
+        <v>554</v>
+      </c>
+      <c r="N79" t="s">
+        <v>555</v>
+      </c>
+      <c r="O79" t="s">
+        <v>556</v>
+      </c>
+      <c r="P79" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>526</v>
+      </c>
+      <c r="R79">
+        <v>0.028664112091064453</v>
+      </c>
+      <c r="S79" t="s">
+        <v>557</v>
+      </c>
+      <c r="T79">
+        <v>0</v>
+      </c>
+      <c r="U79">
+        <v>79</v>
+      </c>
+      <c r="V79">
+        <v>1</v>
+      </c>
+      <c r="W79">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23">
+      <c r="A80">
+        <v>8.0</v>
+      </c>
+      <c r="B80">
+        <v>5.0</v>
+      </c>
+      <c r="C80">
+        <v>1.0</v>
+      </c>
+      <c r="D80">
+        <v>25.0</v>
+      </c>
+      <c r="E80">
+        <v>0.0</v>
+      </c>
+      <c r="F80">
+        <v>100.0</v>
+      </c>
+      <c r="G80">
+        <v>0.0</v>
+      </c>
+      <c r="H80">
+        <v>90.0</v>
+      </c>
+      <c r="I80">
+        <v>0.0</v>
+      </c>
+      <c r="J80" t="s">
+        <v>521</v>
+      </c>
+      <c r="K80">
+        <v>0.01</v>
+      </c>
+      <c r="L80" t="s">
+        <v>558</v>
+      </c>
+      <c r="M80" t="s">
+        <v>559</v>
+      </c>
+      <c r="N80" t="s">
+        <v>560</v>
+      </c>
+      <c r="O80" t="s">
+        <v>561</v>
+      </c>
+      <c r="P80" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>526</v>
+      </c>
+      <c r="R80">
+        <v>108.81562614440918</v>
+      </c>
+      <c r="S80" t="s">
+        <v>562</v>
+      </c>
+      <c r="T80">
+        <v>0</v>
+      </c>
+      <c r="U80">
+        <v>80</v>
+      </c>
+      <c r="V80">
+        <v>1</v>
+      </c>
+      <c r="W80">
+        <v>4826105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23">
+      <c r="A81">
+        <v>8.0</v>
+      </c>
+      <c r="B81">
+        <v>5.0</v>
+      </c>
+      <c r="C81">
+        <v>1.0</v>
+      </c>
+      <c r="D81">
+        <v>25.0</v>
+      </c>
+      <c r="E81">
+        <v>0.0</v>
+      </c>
+      <c r="F81">
+        <v>100.0</v>
+      </c>
+      <c r="G81">
+        <v>0.0</v>
+      </c>
+      <c r="H81">
+        <v>108.0</v>
+      </c>
+      <c r="I81">
+        <v>0.0</v>
+      </c>
+      <c r="J81" t="s">
+        <v>521</v>
+      </c>
+      <c r="K81">
+        <v>0.01</v>
+      </c>
+      <c r="L81" t="s">
+        <v>563</v>
+      </c>
+      <c r="M81" t="s">
+        <v>564</v>
+      </c>
+      <c r="N81" t="s">
+        <v>565</v>
+      </c>
+      <c r="O81" t="s">
+        <v>566</v>
+      </c>
+      <c r="P81" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>526</v>
+      </c>
+      <c r="R81">
+        <v>0.0507969856262207</v>
+      </c>
+      <c r="S81" t="s">
+        <v>567</v>
+      </c>
+      <c r="T81">
+        <v>0</v>
+      </c>
+      <c r="U81">
+        <v>81</v>
+      </c>
+      <c r="V81">
+        <v>1</v>
+      </c>
+      <c r="W81">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23">
+      <c r="A82">
+        <v>8.0</v>
+      </c>
+      <c r="B82">
+        <v>5.0</v>
+      </c>
+      <c r="C82">
+        <v>1.0</v>
+      </c>
+      <c r="D82">
+        <v>25.0</v>
+      </c>
+      <c r="E82">
+        <v>0.0</v>
+      </c>
+      <c r="F82">
+        <v>100.0</v>
+      </c>
+      <c r="G82">
+        <v>0.0</v>
+      </c>
+      <c r="H82">
+        <v>126.0</v>
+      </c>
+      <c r="I82">
+        <v>0.0</v>
+      </c>
+      <c r="J82" t="s">
+        <v>521</v>
+      </c>
+      <c r="K82">
+        <v>0.01</v>
+      </c>
+      <c r="L82" t="s">
+        <v>568</v>
+      </c>
+      <c r="M82" t="s">
+        <v>569</v>
+      </c>
+      <c r="N82" t="s">
+        <v>570</v>
+      </c>
+      <c r="O82" t="s">
+        <v>571</v>
+      </c>
+      <c r="P82" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>526</v>
+      </c>
+      <c r="R82">
+        <v>0.04879403114318848</v>
+      </c>
+      <c r="S82" t="s">
+        <v>572</v>
+      </c>
+      <c r="T82">
+        <v>0</v>
+      </c>
+      <c r="U82">
+        <v>82</v>
+      </c>
+      <c r="V82">
+        <v>1</v>
+      </c>
+      <c r="W82">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23">
+      <c r="A83">
+        <v>8.0</v>
+      </c>
+      <c r="B83">
+        <v>5.0</v>
+      </c>
+      <c r="C83">
+        <v>1.0</v>
+      </c>
+      <c r="D83">
+        <v>25.0</v>
+      </c>
+      <c r="E83">
+        <v>0.0</v>
+      </c>
+      <c r="F83">
+        <v>100.0</v>
+      </c>
+      <c r="G83">
+        <v>0.0</v>
+      </c>
+      <c r="H83">
+        <v>144.0</v>
+      </c>
+      <c r="I83">
+        <v>0.0</v>
+      </c>
+      <c r="J83" t="s">
+        <v>521</v>
+      </c>
+      <c r="K83">
+        <v>0.01</v>
+      </c>
+      <c r="L83" t="s">
+        <v>573</v>
+      </c>
+      <c r="M83" t="s">
+        <v>574</v>
+      </c>
+      <c r="N83" t="s">
+        <v>575</v>
+      </c>
+      <c r="O83" t="s">
+        <v>576</v>
+      </c>
+      <c r="P83" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>526</v>
+      </c>
+      <c r="R83">
+        <v>0.40076303482055664</v>
+      </c>
+      <c r="S83" t="s">
+        <v>577</v>
+      </c>
+      <c r="T83">
+        <v>0</v>
+      </c>
+      <c r="U83">
+        <v>83</v>
+      </c>
+      <c r="V83">
+        <v>1</v>
+      </c>
+      <c r="W83">
+        <v>16704</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23">
+      <c r="A84">
+        <v>8.0</v>
+      </c>
+      <c r="B84">
+        <v>5.0</v>
+      </c>
+      <c r="C84">
+        <v>1.0</v>
+      </c>
+      <c r="D84">
+        <v>25.0</v>
+      </c>
+      <c r="E84">
+        <v>0.0</v>
+      </c>
+      <c r="F84">
+        <v>100.0</v>
+      </c>
+      <c r="G84">
+        <v>0.0</v>
+      </c>
+      <c r="H84">
+        <v>162.0</v>
+      </c>
+      <c r="I84">
+        <v>0.0</v>
+      </c>
+      <c r="J84" t="s">
+        <v>521</v>
+      </c>
+      <c r="K84">
+        <v>0.01</v>
+      </c>
+      <c r="L84" t="s">
+        <v>578</v>
+      </c>
+      <c r="M84" t="s">
+        <v>579</v>
+      </c>
+      <c r="N84" t="s">
+        <v>580</v>
+      </c>
+      <c r="O84" t="s">
+        <v>581</v>
+      </c>
+      <c r="P84" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>526</v>
+      </c>
+      <c r="R84">
+        <v>0.06570792198181152</v>
+      </c>
+      <c r="S84" t="s">
+        <v>582</v>
+      </c>
+      <c r="T84">
+        <v>0</v>
+      </c>
+      <c r="U84">
+        <v>84</v>
+      </c>
+      <c r="V84">
+        <v>1</v>
+      </c>
+      <c r="W84">
+        <v>2378</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23">
+      <c r="A85">
+        <v>8.0</v>
+      </c>
+      <c r="B85">
+        <v>5.0</v>
+      </c>
+      <c r="C85">
+        <v>1.0</v>
+      </c>
+      <c r="D85">
+        <v>25.0</v>
+      </c>
+      <c r="E85">
+        <v>0.0</v>
+      </c>
+      <c r="F85">
+        <v>100.0</v>
+      </c>
+      <c r="G85">
+        <v>0.0</v>
+      </c>
+      <c r="H85">
+        <v>180.0</v>
+      </c>
+      <c r="I85">
+        <v>0.0</v>
+      </c>
+      <c r="J85" t="s">
+        <v>521</v>
+      </c>
+      <c r="K85">
+        <v>0.01</v>
+      </c>
+      <c r="L85" t="s">
+        <v>583</v>
+      </c>
+      <c r="M85" t="s">
+        <v>584</v>
+      </c>
+      <c r="N85" t="s">
+        <v>585</v>
+      </c>
+      <c r="O85" t="s">
+        <v>586</v>
+      </c>
+      <c r="P85" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>526</v>
+      </c>
+      <c r="R85">
+        <v>110.05816006660461</v>
+      </c>
+      <c r="S85" t="s">
+        <v>587</v>
+      </c>
+      <c r="T85">
+        <v>0</v>
+      </c>
+      <c r="U85">
+        <v>85</v>
+      </c>
+      <c r="V85">
+        <v>1</v>
+      </c>
+      <c r="W85">
+        <v>4852042</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23">
+      <c r="A86">
+        <v>8.0</v>
+      </c>
+      <c r="B86">
+        <v>5.0</v>
+      </c>
+      <c r="C86">
+        <v>1.0</v>
+      </c>
+      <c r="D86">
+        <v>25.0</v>
+      </c>
+      <c r="E86">
+        <v>0.0</v>
+      </c>
+      <c r="F86">
+        <v>100.0</v>
+      </c>
+      <c r="G86">
+        <v>0.0</v>
+      </c>
+      <c r="H86">
+        <v>198.0</v>
+      </c>
+      <c r="I86">
+        <v>0.0</v>
+      </c>
+      <c r="J86" t="s">
+        <v>521</v>
+      </c>
+      <c r="K86">
+        <v>0.01</v>
+      </c>
+      <c r="L86" t="s">
+        <v>588</v>
+      </c>
+      <c r="M86" t="s">
+        <v>589</v>
+      </c>
+      <c r="N86" t="s">
+        <v>590</v>
+      </c>
+      <c r="O86" t="s">
+        <v>591</v>
+      </c>
+      <c r="P86" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>526</v>
+      </c>
+      <c r="R86">
+        <v>0.08002805709838867</v>
+      </c>
+      <c r="S86" t="s">
+        <v>592</v>
+      </c>
+      <c r="T86">
+        <v>0</v>
+      </c>
+      <c r="U86">
+        <v>86</v>
+      </c>
+      <c r="V86">
+        <v>1</v>
+      </c>
+      <c r="W86">
+        <v>4717</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23">
+      <c r="A87">
+        <v>8.0</v>
+      </c>
+      <c r="B87">
+        <v>5.0</v>
+      </c>
+      <c r="C87">
+        <v>1.0</v>
+      </c>
+      <c r="D87">
+        <v>25.0</v>
+      </c>
+      <c r="E87">
+        <v>0.0</v>
+      </c>
+      <c r="F87">
+        <v>100.0</v>
+      </c>
+      <c r="G87">
+        <v>0.0</v>
+      </c>
+      <c r="H87">
+        <v>216.0</v>
+      </c>
+      <c r="I87">
+        <v>0.0</v>
+      </c>
+      <c r="J87" t="s">
+        <v>521</v>
+      </c>
+      <c r="K87">
+        <v>0.01</v>
+      </c>
+      <c r="L87" t="s">
+        <v>593</v>
+      </c>
+      <c r="M87" t="s">
+        <v>594</v>
+      </c>
+      <c r="N87" t="s">
+        <v>595</v>
+      </c>
+      <c r="O87" t="s">
+        <v>596</v>
+      </c>
+      <c r="P87" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>526</v>
+      </c>
+      <c r="R87">
+        <v>0.015024900436401367</v>
+      </c>
+      <c r="S87" t="s">
+        <v>597</v>
+      </c>
+      <c r="T87">
+        <v>0</v>
+      </c>
+      <c r="U87">
+        <v>87</v>
+      </c>
+      <c r="V87">
+        <v>1</v>
+      </c>
+      <c r="W87">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23">
+      <c r="A88">
+        <v>8.0</v>
+      </c>
+      <c r="B88">
+        <v>5.0</v>
+      </c>
+      <c r="C88">
+        <v>1.0</v>
+      </c>
+      <c r="D88">
+        <v>25.0</v>
+      </c>
+      <c r="E88">
+        <v>0.0</v>
+      </c>
+      <c r="F88">
+        <v>100.0</v>
+      </c>
+      <c r="G88">
+        <v>0.0</v>
+      </c>
+      <c r="H88">
+        <v>234.0</v>
+      </c>
+      <c r="I88">
+        <v>0.0</v>
+      </c>
+      <c r="J88" t="s">
+        <v>521</v>
+      </c>
+      <c r="K88">
+        <v>0.01</v>
+      </c>
+      <c r="L88" t="s">
+        <v>598</v>
+      </c>
+      <c r="M88" t="s">
+        <v>599</v>
+      </c>
+      <c r="N88" t="s">
+        <v>600</v>
+      </c>
+      <c r="O88" t="s">
+        <v>601</v>
+      </c>
+      <c r="P88" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>526</v>
+      </c>
+      <c r="R88">
+        <v>0.015524148941040039</v>
+      </c>
+      <c r="S88" t="s">
+        <v>602</v>
+      </c>
+      <c r="T88">
+        <v>0</v>
+      </c>
+      <c r="U88">
+        <v>88</v>
+      </c>
+      <c r="V88">
+        <v>1</v>
+      </c>
+      <c r="W88">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23">
+      <c r="A89">
+        <v>8.0</v>
+      </c>
+      <c r="B89">
+        <v>5.0</v>
+      </c>
+      <c r="C89">
+        <v>1.0</v>
+      </c>
+      <c r="D89">
+        <v>25.0</v>
+      </c>
+      <c r="E89">
+        <v>0.0</v>
+      </c>
+      <c r="F89">
+        <v>100.0</v>
+      </c>
+      <c r="G89">
+        <v>0.0</v>
+      </c>
+      <c r="H89">
+        <v>252.0</v>
+      </c>
+      <c r="I89">
+        <v>0.0</v>
+      </c>
+      <c r="J89" t="s">
+        <v>521</v>
+      </c>
+      <c r="K89">
+        <v>0.01</v>
+      </c>
+      <c r="L89" t="s">
+        <v>603</v>
+      </c>
+      <c r="M89" t="s">
+        <v>604</v>
+      </c>
+      <c r="N89" t="s">
+        <v>605</v>
+      </c>
+      <c r="O89" t="s">
+        <v>606</v>
+      </c>
+      <c r="P89" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>526</v>
+      </c>
+      <c r="R89">
+        <v>0.016978979110717773</v>
+      </c>
+      <c r="S89" t="s">
+        <v>607</v>
+      </c>
+      <c r="T89">
+        <v>0</v>
+      </c>
+      <c r="U89">
+        <v>89</v>
+      </c>
+      <c r="V89">
+        <v>1</v>
+      </c>
+      <c r="W89">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23">
+      <c r="A90">
+        <v>8.0</v>
+      </c>
+      <c r="B90">
+        <v>5.0</v>
+      </c>
+      <c r="C90">
+        <v>1.0</v>
+      </c>
+      <c r="D90">
+        <v>25.0</v>
+      </c>
+      <c r="E90">
+        <v>0.0</v>
+      </c>
+      <c r="F90">
+        <v>100.0</v>
+      </c>
+      <c r="G90">
+        <v>0.0</v>
+      </c>
+      <c r="H90">
+        <v>270.0</v>
+      </c>
+      <c r="I90">
+        <v>0.0</v>
+      </c>
+      <c r="J90" t="s">
+        <v>521</v>
+      </c>
+      <c r="K90">
+        <v>0.01</v>
+      </c>
+      <c r="L90" t="s">
+        <v>608</v>
+      </c>
+      <c r="M90" t="s">
+        <v>609</v>
+      </c>
+      <c r="N90" t="s">
+        <v>610</v>
+      </c>
+      <c r="O90" t="s">
+        <v>611</v>
+      </c>
+      <c r="P90" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>526</v>
+      </c>
+      <c r="R90">
+        <v>71.28549599647522</v>
+      </c>
+      <c r="S90" t="s">
+        <v>612</v>
+      </c>
+      <c r="T90">
+        <v>0</v>
+      </c>
+      <c r="U90">
+        <v>90</v>
+      </c>
+      <c r="V90">
+        <v>1</v>
+      </c>
+      <c r="W90">
+        <v>4826105</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23">
+      <c r="A91">
+        <v>8.0</v>
+      </c>
+      <c r="B91">
+        <v>5.0</v>
+      </c>
+      <c r="C91">
+        <v>1.0</v>
+      </c>
+      <c r="D91">
+        <v>25.0</v>
+      </c>
+      <c r="E91">
+        <v>0.0</v>
+      </c>
+      <c r="F91">
+        <v>100.0</v>
+      </c>
+      <c r="G91">
+        <v>0.0</v>
+      </c>
+      <c r="H91">
+        <v>288.0</v>
+      </c>
+      <c r="I91">
+        <v>0.0</v>
+      </c>
+      <c r="J91" t="s">
+        <v>521</v>
+      </c>
+      <c r="K91">
+        <v>0.01</v>
+      </c>
+      <c r="L91" t="s">
+        <v>613</v>
+      </c>
+      <c r="M91" t="s">
+        <v>614</v>
+      </c>
+      <c r="N91" t="s">
+        <v>615</v>
+      </c>
+      <c r="O91" t="s">
+        <v>616</v>
+      </c>
+      <c r="P91" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>526</v>
+      </c>
+      <c r="R91">
+        <v>0.037629127502441406</v>
+      </c>
+      <c r="S91" t="s">
+        <v>617</v>
+      </c>
+      <c r="T91">
+        <v>0</v>
+      </c>
+      <c r="U91">
+        <v>91</v>
+      </c>
+      <c r="V91">
+        <v>1</v>
+      </c>
+      <c r="W91">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23">
+      <c r="A92">
+        <v>8.0</v>
+      </c>
+      <c r="B92">
+        <v>5.0</v>
+      </c>
+      <c r="C92">
+        <v>1.0</v>
+      </c>
+      <c r="D92">
+        <v>25.0</v>
+      </c>
+      <c r="E92">
+        <v>0.0</v>
+      </c>
+      <c r="F92">
+        <v>100.0</v>
+      </c>
+      <c r="G92">
+        <v>0.0</v>
+      </c>
+      <c r="H92">
+        <v>306.0</v>
+      </c>
+      <c r="I92">
+        <v>0.0</v>
+      </c>
+      <c r="J92" t="s">
+        <v>521</v>
+      </c>
+      <c r="K92">
+        <v>0.01</v>
+      </c>
+      <c r="L92" t="s">
+        <v>618</v>
+      </c>
+      <c r="M92" t="s">
+        <v>619</v>
+      </c>
+      <c r="N92" t="s">
+        <v>620</v>
+      </c>
+      <c r="O92" t="s">
+        <v>621</v>
+      </c>
+      <c r="P92" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>526</v>
+      </c>
+      <c r="R92">
+        <v>0.0482330322265625</v>
+      </c>
+      <c r="S92" t="s">
+        <v>622</v>
+      </c>
+      <c r="T92">
+        <v>0</v>
+      </c>
+      <c r="U92">
+        <v>92</v>
+      </c>
+      <c r="V92">
+        <v>1</v>
+      </c>
+      <c r="W92">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23">
+      <c r="A93">
+        <v>8.0</v>
+      </c>
+      <c r="B93">
+        <v>5.0</v>
+      </c>
+      <c r="C93">
+        <v>1.0</v>
+      </c>
+      <c r="D93">
+        <v>25.0</v>
+      </c>
+      <c r="E93">
+        <v>0.0</v>
+      </c>
+      <c r="F93">
+        <v>100.0</v>
+      </c>
+      <c r="G93">
+        <v>0.0</v>
+      </c>
+      <c r="H93">
+        <v>324.0</v>
+      </c>
+      <c r="I93">
+        <v>0.0</v>
+      </c>
+      <c r="J93" t="s">
+        <v>521</v>
+      </c>
+      <c r="K93">
+        <v>0.01</v>
+      </c>
+      <c r="L93" t="s">
+        <v>623</v>
+      </c>
+      <c r="M93" t="s">
+        <v>624</v>
+      </c>
+      <c r="N93" t="s">
+        <v>625</v>
+      </c>
+      <c r="O93" t="s">
+        <v>626</v>
+      </c>
+      <c r="P93" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>526</v>
+      </c>
+      <c r="R93">
+        <v>0.0536189079284668</v>
+      </c>
+      <c r="S93" t="s">
+        <v>627</v>
+      </c>
+      <c r="T93">
+        <v>0</v>
+      </c>
+      <c r="U93">
+        <v>93</v>
+      </c>
+      <c r="V93">
+        <v>1</v>
+      </c>
+      <c r="W93">
+        <v>2996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23">
+      <c r="A94">
+        <v>8.0</v>
+      </c>
+      <c r="B94">
+        <v>5.0</v>
+      </c>
+      <c r="C94">
+        <v>1.0</v>
+      </c>
+      <c r="D94">
+        <v>25.0</v>
+      </c>
+      <c r="E94">
+        <v>0.0</v>
+      </c>
+      <c r="F94">
+        <v>100.0</v>
+      </c>
+      <c r="G94">
+        <v>0.0</v>
+      </c>
+      <c r="H94">
+        <v>342.0</v>
+      </c>
+      <c r="I94">
+        <v>0.0</v>
+      </c>
+      <c r="J94" t="s">
+        <v>521</v>
+      </c>
+      <c r="K94">
+        <v>0.01</v>
+      </c>
+      <c r="L94" t="s">
+        <v>628</v>
+      </c>
+      <c r="M94" t="s">
+        <v>629</v>
+      </c>
+      <c r="N94" t="s">
+        <v>630</v>
+      </c>
+      <c r="O94" t="s">
+        <v>631</v>
+      </c>
+      <c r="P94" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>526</v>
+      </c>
+      <c r="R94">
+        <v>0.03743696212768555</v>
+      </c>
+      <c r="S94" t="s">
+        <v>632</v>
+      </c>
+      <c r="T94">
+        <v>0</v>
+      </c>
+      <c r="U94">
+        <v>94</v>
+      </c>
+      <c r="V94">
+        <v>1</v>
+      </c>
+      <c r="W94">
+        <v>1900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>